<commit_message>
work on DMM list and wiki
</commit_message>
<xml_diff>
--- a/DMM.xlsx
+++ b/DMM.xlsx
@@ -2,20 +2,23 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15480" windowHeight="10005" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="15480" windowHeight="10005" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration" sheetId="2" r:id="rId1"/>
-    <sheet name="Tabelle1" sheetId="11" r:id="rId2"/>
-    <sheet name="Tabelle2" sheetId="12" r:id="rId3"/>
-    <sheet name="Tabelle3" sheetId="13" r:id="rId4"/>
+    <sheet name="Gadget-DMM" sheetId="11" r:id="rId2"/>
+    <sheet name="Gadget-GasSer" sheetId="12" r:id="rId3"/>
+    <sheet name="Gadget-Dust" sheetId="13" r:id="rId4"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Gadget-DMM'!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Gadget-Dust'!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Gadget-GasSer'!$A$1:$G$1</definedName>
     <definedName name="Suchkriterien0">[1]Lieferschein!#REF!</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -57,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="211">
   <si>
     <t>yes</t>
   </si>
@@ -264,129 +267,6 @@
     <t>Kommentar</t>
   </si>
   <si>
-    <t xml:space="preserve">Criteria </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Issue Status </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search based in issue statuses </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Priority </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Issue Types </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search All </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Used with keyword search </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subject </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solution </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not Used at present </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Version Number </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product Version Number </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product Name </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Specific product as supported by teleSys. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Environment </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date Opened </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date Closed </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Time Open </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not used at present </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adj Time Open </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Labor hours </t>
-  </si>
-  <si>
-    <t>Issue Sub-status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Issue priorities: CRITICAL, MAJOR, MINOR and FYI. 
-Defined in Table 1: Issue Submission Criteria. </t>
-  </si>
-  <si>
-    <t>Used to search based on specific subject; which has been entered while logging the issue.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Environment setup: 
-- Evaluation 
-- Development &amp; Integration 
-- Engineering Test 
-- QA Test 
-- Field Trial 
-- Inter-operability Test (IOT) 
-- Network Deployment 
-Defined in Table 1: Issue Submission Criteria. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Types of issue: 
-- Software Issues 
-- Software Installation 
-- Software OAM&amp;P 
-- Software Maintenance 
-- Software Enhancement 
-- Operating System 
-- Hardware Network Card Issues 
-- Hardware Network Card Enhancements 
-- Hardware Server Node 
-- System 
-- Network 
-- Documentation 
-- Logistics 
-Defined in Table 1: Issue Submission Criteria. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search based in issue sub-statuses: 
-- Under Investigation: Issue is under investigation 
-- Fixed with QA: Issue has been fixed and under QA test 
-- Resolved: Issue has been resolved and pending confirmation from 
-customer. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Used to search based on specific notes; which has been entered while logging or updating the issue. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Used to define Start Date and End Date between which the required issues have been logged. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Used to define Start Date and End Date between which the required issues have been Closed. </t>
-  </si>
-  <si>
     <t>Manufacurer</t>
   </si>
   <si>
@@ -775,6 +655,126 @@
   </si>
   <si>
     <t>VC 940</t>
+  </si>
+  <si>
+    <t>Winsen</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>MH-Z14A</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>MH-Z19</t>
+  </si>
+  <si>
+    <t>5000 ppm</t>
+  </si>
+  <si>
+    <t>ZE07-CO</t>
+  </si>
+  <si>
+    <t>5 mg/m3</t>
+  </si>
+  <si>
+    <t>ZE08-CH2O</t>
+  </si>
+  <si>
+    <t>CH2O (Formaldehyde)</t>
+  </si>
+  <si>
+    <t>CO (Carbo Monoxide)</t>
+  </si>
+  <si>
+    <t>CO2 (Carbo Dioxide)</t>
+  </si>
+  <si>
+    <t>SDS011</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>SDS01x</t>
+  </si>
+  <si>
+    <t>Nova Fitness</t>
+  </si>
+  <si>
+    <t>SDS018</t>
+  </si>
+  <si>
+    <t>SDS189</t>
+  </si>
+  <si>
+    <t>PM100</t>
+  </si>
+  <si>
+    <t>SDS198</t>
+  </si>
+  <si>
+    <t>Plantower</t>
+  </si>
+  <si>
+    <t>PMS5003</t>
+  </si>
+  <si>
+    <t>PMSx003</t>
+  </si>
+  <si>
+    <t>PMS7003</t>
+  </si>
+  <si>
+    <t>PM2.5, PM10</t>
+  </si>
+  <si>
+    <t>PM1, PM2.5, PM10</t>
+  </si>
+  <si>
+    <t>GDPID</t>
+  </si>
+  <si>
+    <t>Plugin Name</t>
+  </si>
+  <si>
+    <t>Dust Sensor PMS5003/7003</t>
+  </si>
+  <si>
+    <t>gdDust_PMSx003</t>
+  </si>
+  <si>
+    <t>gdDust_SDS01x</t>
+  </si>
+  <si>
+    <t>Dust Sensor SDS011/018</t>
+  </si>
+  <si>
+    <t>Dust Sensor SDS198</t>
+  </si>
+  <si>
+    <t>gdDust_SDS198</t>
+  </si>
+  <si>
+    <t>gdGasSer_WinsenPoll</t>
+  </si>
+  <si>
+    <t>Gas Winsen Poll (UART)</t>
+  </si>
+  <si>
+    <t>gdGasSer_WinsenActive</t>
+  </si>
+  <si>
+    <t>Gas Winsen Active (UART)</t>
+  </si>
+  <si>
+    <t>WinsenActive</t>
+  </si>
+  <si>
+    <t>WinsenPoll</t>
   </si>
 </sst>
 </file>
@@ -1963,7 +1963,7 @@
   <dimension ref="B2:N38"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -2078,7 +2078,7 @@
         <v>4</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="2"/>
@@ -2092,7 +2092,7 @@
         <v>5</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="2"/>
@@ -2158,7 +2158,7 @@
         <v>24</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E20" s="14"/>
       <c r="G20" s="19" t="s">
@@ -2249,7 +2249,7 @@
       </c>
       <c r="D32" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>no</v>
+        <v>yes</v>
       </c>
       <c r="G32" s="38" t="s">
         <v>30</v>
@@ -2268,7 +2268,7 @@
       </c>
       <c r="D33" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>no</v>
+        <v>yes</v>
       </c>
       <c r="G33" s="38" t="s">
         <v>30</v>
@@ -2323,7 +2323,7 @@
       </c>
       <c r="D38" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>yes</v>
+        <v>no</v>
       </c>
     </row>
   </sheetData>
@@ -2362,8 +2362,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2380,39 +2380,39 @@
   <sheetData>
     <row r="1" spans="1:7" s="49" customFormat="1">
       <c r="A1" s="48" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="B1" s="48" t="s">
         <v>39</v>
       </c>
       <c r="C1" s="48" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="D1" s="48" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="E1" s="48" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="F1" s="48" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="G1" s="49" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="50" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="D2" s="51" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="E2" s="50" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="F2" s="50">
         <v>1</v>
@@ -2420,16 +2420,16 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="50" t="s">
-        <v>83</v>
+        <v>51</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="D3" s="51" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="E3" s="50" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="F3" s="50">
         <v>1</v>
@@ -2437,16 +2437,16 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="50" t="s">
-        <v>83</v>
+        <v>51</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="F4" s="50">
         <v>1</v>
@@ -2454,16 +2454,16 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="50" t="s">
-        <v>83</v>
+        <v>51</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="D5" s="51" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="E5" s="50" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="F5" s="50">
         <v>1</v>
@@ -2471,16 +2471,16 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="50" t="s">
-        <v>83</v>
+        <v>51</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
       <c r="D6" s="51" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="E6" s="50" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="F6" s="50">
         <v>1</v>
@@ -2488,16 +2488,16 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="50" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
       <c r="D7" s="51" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="E7" s="50" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="F7" s="50">
         <v>1</v>
@@ -2505,16 +2505,16 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="50" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="D8" s="50" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="E8" s="50" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="F8" s="50">
         <v>1</v>
@@ -2522,19 +2522,19 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="50" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="C9" s="50" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="D9" s="53" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="E9" s="50" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="F9" s="50">
         <v>2</v>
@@ -2542,16 +2542,16 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="50" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="B10" s="50">
         <v>95</v>
       </c>
       <c r="D10" s="50" t="s">
-        <v>101</v>
+        <v>69</v>
       </c>
       <c r="E10" s="50" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="F10" s="50">
         <v>1</v>
@@ -2559,16 +2559,16 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="50" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="B11" s="50">
         <v>97</v>
       </c>
       <c r="D11" s="50" t="s">
-        <v>101</v>
+        <v>69</v>
       </c>
       <c r="E11" s="50" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="F11" s="50">
         <v>1</v>
@@ -2576,39 +2576,39 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="50" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="B12" s="50" t="s">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="C12" s="50" t="s">
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="D12" s="51" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="E12" s="50" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="F12" s="50">
         <v>1</v>
       </c>
       <c r="G12" s="50" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="50" t="s">
-        <v>107</v>
+        <v>75</v>
       </c>
       <c r="B13" s="50" t="s">
-        <v>108</v>
+        <v>76</v>
       </c>
       <c r="D13" s="50" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="E13" s="50" t="s">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="F13" s="50">
         <v>1</v>
@@ -2616,16 +2616,16 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="50" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="B14" s="50" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="D14" s="50" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="E14" s="50" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="F14" s="50">
         <v>1</v>
@@ -2633,16 +2633,16 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="50" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="B15" s="50" t="s">
-        <v>112</v>
+        <v>80</v>
       </c>
       <c r="D15" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E15" s="50" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="F15" s="50">
         <v>1</v>
@@ -2650,16 +2650,16 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="50" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="B16" s="50" t="s">
-        <v>113</v>
+        <v>81</v>
       </c>
       <c r="D16" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E16" s="50" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="F16" s="50">
         <v>1</v>
@@ -2667,39 +2667,39 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="50" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="B17" s="50" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="C17" s="50" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="E17" s="50" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="F17" s="50">
         <v>2</v>
       </c>
       <c r="G17" s="50" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="50" t="s">
-        <v>114</v>
+        <v>82</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>115</v>
+        <v>83</v>
       </c>
       <c r="D18" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E18" s="50" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="F18" s="50">
         <v>1</v>
@@ -2707,16 +2707,16 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="50" t="s">
-        <v>114</v>
+        <v>82</v>
       </c>
       <c r="B19" s="50" t="s">
-        <v>116</v>
+        <v>84</v>
       </c>
       <c r="D19" s="50" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="E19" s="50" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="F19" s="50">
         <v>1</v>
@@ -2724,16 +2724,16 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="50" t="s">
-        <v>117</v>
+        <v>85</v>
       </c>
       <c r="B20" s="50" t="s">
-        <v>118</v>
+        <v>86</v>
       </c>
       <c r="D20" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E20" s="50" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="F20" s="50">
         <v>1</v>
@@ -2741,16 +2741,16 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="50" t="s">
-        <v>117</v>
+        <v>85</v>
       </c>
       <c r="B21" s="50" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
       <c r="D21" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E21" s="50" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="F21" s="50">
         <v>4</v>
@@ -2758,16 +2758,16 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="50" t="s">
-        <v>117</v>
+        <v>85</v>
       </c>
       <c r="B22" s="50" t="s">
-        <v>121</v>
+        <v>89</v>
       </c>
       <c r="D22" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E22" s="50" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="F22" s="50">
         <v>4</v>
@@ -2775,16 +2775,16 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="50" t="s">
-        <v>117</v>
+        <v>85</v>
       </c>
       <c r="B23" s="50" t="s">
-        <v>122</v>
+        <v>90</v>
       </c>
       <c r="D23" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E23" s="50" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="F23" s="50">
         <v>4</v>
@@ -2792,16 +2792,16 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="50" t="s">
-        <v>117</v>
+        <v>85</v>
       </c>
       <c r="B24" s="50" t="s">
-        <v>123</v>
+        <v>91</v>
       </c>
       <c r="D24" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E24" s="50" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="F24" s="50">
         <v>4</v>
@@ -2809,16 +2809,16 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="50" t="s">
-        <v>117</v>
+        <v>85</v>
       </c>
       <c r="B25" s="50" t="s">
-        <v>125</v>
+        <v>93</v>
       </c>
       <c r="D25" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E25" s="50" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="F25" s="50">
         <v>4</v>
@@ -2826,16 +2826,16 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="50" t="s">
-        <v>117</v>
+        <v>85</v>
       </c>
       <c r="B26" s="50" t="s">
-        <v>126</v>
+        <v>94</v>
       </c>
       <c r="D26" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E26" s="50" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="F26" s="50">
         <v>4</v>
@@ -2843,16 +2843,16 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="50" t="s">
-        <v>117</v>
+        <v>85</v>
       </c>
       <c r="B27" s="50" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="D27" s="50" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="E27" s="50" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="F27" s="50">
         <v>1</v>
@@ -2860,16 +2860,16 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="50" t="s">
-        <v>117</v>
+        <v>85</v>
       </c>
       <c r="B28" s="50" t="s">
-        <v>127</v>
+        <v>95</v>
       </c>
       <c r="D28" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E28" s="50" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="F28" s="50">
         <v>1</v>
@@ -2877,16 +2877,16 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="50" t="s">
-        <v>117</v>
+        <v>85</v>
       </c>
       <c r="B29" s="50" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="D29" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E29" s="50" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="F29" s="50">
         <v>1</v>
@@ -2894,16 +2894,16 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="50" t="s">
-        <v>117</v>
+        <v>85</v>
       </c>
       <c r="B30" s="50" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
       <c r="D30" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E30" s="50" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="F30" s="50">
         <v>1</v>
@@ -2911,16 +2911,16 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="50" t="s">
-        <v>117</v>
+        <v>85</v>
       </c>
       <c r="B31" s="50" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
       <c r="D31" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E31" s="50" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="F31" s="50">
         <v>1</v>
@@ -2928,16 +2928,16 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="50" t="s">
-        <v>117</v>
+        <v>85</v>
       </c>
       <c r="B32" s="50" t="s">
-        <v>131</v>
+        <v>99</v>
       </c>
       <c r="D32" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E32" s="50" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="F32" s="50">
         <v>1</v>
@@ -2945,19 +2945,19 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="50" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
       <c r="B33" s="50" t="s">
-        <v>133</v>
+        <v>101</v>
       </c>
       <c r="C33" s="50" t="s">
-        <v>134</v>
+        <v>102</v>
       </c>
       <c r="D33" s="54" t="s">
-        <v>135</v>
+        <v>103</v>
       </c>
       <c r="E33" s="50" t="s">
-        <v>136</v>
+        <v>104</v>
       </c>
       <c r="F33" s="50">
         <v>1</v>
@@ -2965,16 +2965,16 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="50" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="B34" s="50">
         <v>451</v>
       </c>
       <c r="D34" s="50" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
       <c r="E34" s="50" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="F34" s="50">
         <v>1</v>
@@ -2982,16 +2982,16 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="50" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="B35" s="50">
         <v>3330</v>
       </c>
       <c r="D35" s="51" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="E35" s="50" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="F35" s="50">
         <v>1</v>
@@ -2999,19 +2999,19 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="50" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="B36" s="50">
         <v>4000</v>
       </c>
       <c r="C36" s="50" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="D36" s="53" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="E36" s="50" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="F36" s="50">
         <v>2</v>
@@ -3019,16 +3019,16 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="50" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="B37" s="50">
         <v>4010</v>
       </c>
       <c r="D37" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E37" s="50" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="F37" s="50">
         <v>1</v>
@@ -3036,16 +3036,16 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="50" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="B38" s="50">
         <v>4360</v>
       </c>
       <c r="D38" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E38" s="50" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="F38" s="50">
         <v>1</v>
@@ -3053,16 +3053,16 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="50" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="B39" s="50">
         <v>4365</v>
       </c>
       <c r="D39" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E39" s="50" t="s">
-        <v>139</v>
+        <v>107</v>
       </c>
       <c r="F39" s="50">
         <v>1</v>
@@ -3070,16 +3070,16 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="50" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="B40" s="50">
         <v>4390</v>
       </c>
       <c r="D40" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E40" s="50" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="F40" s="50">
         <v>4</v>
@@ -3087,16 +3087,16 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="50" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="B41" s="50" t="s">
-        <v>140</v>
+        <v>108</v>
       </c>
       <c r="D41" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E41" s="50" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="F41" s="50">
         <v>4</v>
@@ -3104,16 +3104,16 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="50" t="s">
-        <v>141</v>
+        <v>109</v>
       </c>
       <c r="B42" s="50" t="s">
-        <v>142</v>
+        <v>110</v>
       </c>
       <c r="D42" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E42" s="50" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="F42" s="50">
         <v>1</v>
@@ -3121,16 +3121,16 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="50" t="s">
-        <v>141</v>
+        <v>109</v>
       </c>
       <c r="B43" s="50" t="s">
-        <v>143</v>
+        <v>111</v>
       </c>
       <c r="D43" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E43" s="50" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="F43" s="50">
         <v>1</v>
@@ -3138,16 +3138,16 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>144</v>
+        <v>112</v>
       </c>
       <c r="B44" s="50" t="s">
-        <v>112</v>
+        <v>80</v>
       </c>
       <c r="D44" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E44" s="50" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="F44" s="50">
         <v>1</v>
@@ -3155,19 +3155,19 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="50" t="s">
-        <v>144</v>
+        <v>112</v>
       </c>
       <c r="B45" s="50" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="C45" s="50" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="D45" s="53" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="E45" s="50" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="F45" s="50">
         <v>2</v>
@@ -3175,16 +3175,16 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="50" t="s">
-        <v>145</v>
+        <v>113</v>
       </c>
       <c r="B46" s="50" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="D46" s="51" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="E46" s="50" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="F46" s="50">
         <v>1</v>
@@ -3192,16 +3192,16 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="50" t="s">
-        <v>147</v>
+        <v>115</v>
       </c>
       <c r="B47" s="50" t="s">
-        <v>148</v>
+        <v>116</v>
       </c>
       <c r="D47" s="51" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="E47" s="50" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="F47" s="50">
         <v>1</v>
@@ -3209,16 +3209,16 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="50" t="s">
-        <v>147</v>
+        <v>115</v>
       </c>
       <c r="B48" s="50" t="s">
-        <v>149</v>
+        <v>117</v>
       </c>
       <c r="D48" s="51" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="E48" s="50" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="F48" s="50">
         <v>1</v>
@@ -3226,19 +3226,19 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="50" t="s">
-        <v>147</v>
+        <v>115</v>
       </c>
       <c r="B49" s="50" t="s">
-        <v>150</v>
+        <v>118</v>
       </c>
       <c r="C49" s="50" t="s">
-        <v>134</v>
+        <v>102</v>
       </c>
       <c r="D49" s="51" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="E49" s="50" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="F49" s="50">
         <v>1</v>
@@ -3246,19 +3246,19 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="50" t="s">
-        <v>147</v>
+        <v>115</v>
       </c>
       <c r="B50" s="50" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
       <c r="C50" s="50" t="s">
-        <v>134</v>
+        <v>102</v>
       </c>
       <c r="D50" s="51" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="E50" s="50" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="F50" s="50">
         <v>1</v>
@@ -3266,42 +3266,42 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="50" t="s">
-        <v>147</v>
+        <v>115</v>
       </c>
       <c r="B51" s="50" t="s">
-        <v>152</v>
+        <v>120</v>
       </c>
       <c r="C51" s="50" t="s">
-        <v>134</v>
+        <v>102</v>
       </c>
       <c r="D51" s="51" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="E51" s="50" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="F51" s="50">
         <v>1</v>
       </c>
       <c r="G51" s="50" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="50" t="s">
-        <v>147</v>
+        <v>115</v>
       </c>
       <c r="B52" s="50" t="s">
-        <v>153</v>
+        <v>121</v>
       </c>
       <c r="C52" s="50" t="s">
-        <v>134</v>
+        <v>102</v>
       </c>
       <c r="D52" s="51" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="E52" s="50" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="F52" s="50">
         <v>1</v>
@@ -3309,19 +3309,19 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="50" t="s">
-        <v>147</v>
+        <v>115</v>
       </c>
       <c r="B53" s="50" t="s">
-        <v>154</v>
+        <v>122</v>
       </c>
       <c r="C53" s="50" t="s">
-        <v>134</v>
+        <v>102</v>
       </c>
       <c r="D53" s="51" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="E53" s="50" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="F53" s="50">
         <v>1</v>
@@ -3329,39 +3329,39 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="50" t="s">
-        <v>147</v>
+        <v>115</v>
       </c>
       <c r="B54" s="50" t="s">
-        <v>133</v>
+        <v>101</v>
       </c>
       <c r="C54" s="50" t="s">
-        <v>134</v>
+        <v>102</v>
       </c>
       <c r="D54" s="54" t="s">
-        <v>135</v>
+        <v>103</v>
       </c>
       <c r="E54" s="50" t="s">
-        <v>136</v>
+        <v>104</v>
       </c>
       <c r="F54" s="50">
         <v>1</v>
       </c>
       <c r="G54" s="50" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="50" t="s">
-        <v>147</v>
+        <v>115</v>
       </c>
       <c r="B55" s="50" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="D55" s="55" t="s">
-        <v>157</v>
+        <v>125</v>
       </c>
       <c r="E55" s="50" t="s">
-        <v>158</v>
+        <v>126</v>
       </c>
       <c r="F55" s="50">
         <v>1</v>
@@ -3369,16 +3369,16 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="50" t="s">
-        <v>147</v>
+        <v>115</v>
       </c>
       <c r="B56" s="50" t="s">
-        <v>159</v>
+        <v>127</v>
       </c>
       <c r="D56" s="55" t="s">
-        <v>157</v>
+        <v>125</v>
       </c>
       <c r="E56" s="50" t="s">
-        <v>158</v>
+        <v>126</v>
       </c>
       <c r="F56" s="50">
         <v>1</v>
@@ -3386,16 +3386,16 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="50" t="s">
-        <v>160</v>
+        <v>128</v>
       </c>
       <c r="B57" s="50" t="s">
-        <v>161</v>
+        <v>129</v>
       </c>
       <c r="D57" s="51" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="E57" s="50" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="F57" s="50">
         <v>1</v>
@@ -3403,16 +3403,16 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="50" t="s">
-        <v>162</v>
+        <v>130</v>
       </c>
       <c r="B58" s="50" t="s">
-        <v>163</v>
+        <v>131</v>
       </c>
       <c r="D58" s="51" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="E58" s="50" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="F58" s="50">
         <v>1</v>
@@ -3420,16 +3420,16 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="50" t="s">
-        <v>162</v>
+        <v>130</v>
       </c>
       <c r="B59" s="50" t="s">
-        <v>164</v>
+        <v>132</v>
       </c>
       <c r="D59" s="51" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="E59" s="50" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="F59" s="50">
         <v>1</v>
@@ -3437,16 +3437,16 @@
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="50" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="B60" s="50" t="s">
-        <v>166</v>
+        <v>134</v>
       </c>
       <c r="D60" s="50" t="s">
-        <v>167</v>
+        <v>135</v>
       </c>
       <c r="E60" s="50" t="s">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="F60" s="50">
         <v>2</v>
@@ -3454,16 +3454,16 @@
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="50" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="B61" s="50" t="s">
-        <v>168</v>
+        <v>136</v>
       </c>
       <c r="D61" s="50" t="s">
-        <v>167</v>
+        <v>135</v>
       </c>
       <c r="E61" s="50" t="s">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="F61" s="50">
         <v>2</v>
@@ -3471,16 +3471,16 @@
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="50" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="B62" s="50" t="s">
-        <v>169</v>
+        <v>137</v>
       </c>
       <c r="D62" s="50" t="s">
-        <v>167</v>
+        <v>135</v>
       </c>
       <c r="E62" s="50" t="s">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="F62" s="50">
         <v>2</v>
@@ -3488,16 +3488,16 @@
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="50" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="B63" s="50" t="s">
-        <v>170</v>
+        <v>138</v>
       </c>
       <c r="D63" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E63" s="50" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="F63" s="50">
         <v>1</v>
@@ -3505,16 +3505,16 @@
     </row>
     <row r="64" spans="1:7">
       <c r="A64" s="50" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="B64" s="50" t="s">
-        <v>171</v>
+        <v>139</v>
       </c>
       <c r="D64" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E64" s="50" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="F64" s="50">
         <v>1</v>
@@ -3522,16 +3522,16 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="50" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="B65" s="50" t="s">
-        <v>172</v>
+        <v>140</v>
       </c>
       <c r="D65" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E65" s="50" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="F65" s="50">
         <v>1</v>
@@ -3539,16 +3539,16 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="50" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="B66" s="50" t="s">
-        <v>173</v>
+        <v>141</v>
       </c>
       <c r="D66" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E66" s="50" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="F66" s="50">
         <v>1</v>
@@ -3556,16 +3556,16 @@
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="50" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="B67" s="50" t="s">
-        <v>174</v>
+        <v>142</v>
       </c>
       <c r="D67" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E67" s="50" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="F67" s="50">
         <v>4</v>
@@ -3573,16 +3573,16 @@
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="50" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="B68" s="50" t="s">
-        <v>175</v>
+        <v>143</v>
       </c>
       <c r="D68" s="56" t="s">
-        <v>176</v>
+        <v>144</v>
       </c>
       <c r="E68" s="50" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="F68" s="50">
         <v>1</v>
@@ -3590,16 +3590,16 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="50" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="B69" s="50" t="s">
-        <v>177</v>
+        <v>145</v>
       </c>
       <c r="D69" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E69" s="50" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="F69" s="50">
         <v>4</v>
@@ -3607,16 +3607,16 @@
     </row>
     <row r="70" spans="1:6">
       <c r="A70" s="50" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="B70" s="50" t="s">
-        <v>178</v>
+        <v>146</v>
       </c>
       <c r="D70" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E70" s="50" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="F70" s="50">
         <v>4</v>
@@ -3624,16 +3624,16 @@
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="50" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="B71" s="50" t="s">
-        <v>179</v>
+        <v>147</v>
       </c>
       <c r="D71" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E71" s="50" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="F71" s="50">
         <v>4</v>
@@ -3641,16 +3641,16 @@
     </row>
     <row r="72" spans="1:6">
       <c r="A72" s="50" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="B72" s="50" t="s">
-        <v>127</v>
+        <v>95</v>
       </c>
       <c r="D72" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E72" s="50" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="F72" s="50">
         <v>1</v>
@@ -3658,16 +3658,16 @@
     </row>
     <row r="73" spans="1:6">
       <c r="A73" s="50" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="B73" s="50" t="s">
-        <v>180</v>
+        <v>148</v>
       </c>
       <c r="D73" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E73" s="50" t="s">
-        <v>181</v>
+        <v>149</v>
       </c>
       <c r="F73" s="50">
         <v>1</v>
@@ -3675,16 +3675,16 @@
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="50" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="B74" s="50" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
       <c r="D74" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E74" s="50" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="F74" s="50">
         <v>1</v>
@@ -3692,16 +3692,16 @@
     </row>
     <row r="75" spans="1:6">
       <c r="A75" s="50" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="B75" s="50" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
       <c r="D75" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E75" s="50" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="F75" s="50">
         <v>1</v>
@@ -3709,16 +3709,16 @@
     </row>
     <row r="76" spans="1:6">
       <c r="A76" s="50" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="B76" s="50" t="s">
-        <v>182</v>
+        <v>150</v>
       </c>
       <c r="D76" s="52" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E76" s="50" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="F76" s="50">
         <v>4</v>
@@ -3726,16 +3726,16 @@
     </row>
     <row r="77" spans="1:6">
       <c r="A77" s="50" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="B77" s="50" t="s">
-        <v>183</v>
+        <v>151</v>
       </c>
       <c r="D77" s="56" t="s">
-        <v>176</v>
+        <v>144</v>
       </c>
       <c r="E77" s="50" t="s">
-        <v>184</v>
+        <v>152</v>
       </c>
       <c r="F77" s="50">
         <v>1</v>
@@ -3743,16 +3743,16 @@
     </row>
     <row r="78" spans="1:6">
       <c r="A78" s="50" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="B78" s="50" t="s">
-        <v>185</v>
+        <v>153</v>
       </c>
       <c r="D78" s="57" t="s">
-        <v>186</v>
+        <v>154</v>
       </c>
       <c r="E78" s="50" t="s">
-        <v>187</v>
+        <v>155</v>
       </c>
       <c r="F78" s="50">
         <v>1</v>
@@ -3760,16 +3760,16 @@
     </row>
     <row r="79" spans="1:6">
       <c r="A79" s="50" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="B79" s="50" t="s">
-        <v>188</v>
+        <v>156</v>
       </c>
       <c r="D79" s="56" t="s">
-        <v>176</v>
+        <v>144</v>
       </c>
       <c r="E79" s="50" t="s">
-        <v>184</v>
+        <v>152</v>
       </c>
       <c r="F79" s="50">
         <v>1</v>
@@ -3777,33 +3777,33 @@
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="50" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="B80" s="50" t="s">
-        <v>189</v>
+        <v>157</v>
       </c>
       <c r="C80" s="50" t="s">
-        <v>190</v>
+        <v>158</v>
       </c>
       <c r="D80" s="50" t="s">
-        <v>191</v>
+        <v>159</v>
       </c>
       <c r="E80" s="50" t="s">
-        <v>192</v>
+        <v>160</v>
       </c>
     </row>
     <row r="81" spans="1:7">
       <c r="A81" s="50" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="B81" s="50" t="s">
-        <v>193</v>
+        <v>161</v>
       </c>
       <c r="D81" s="57" t="s">
-        <v>186</v>
+        <v>154</v>
       </c>
       <c r="E81" s="50" t="s">
-        <v>187</v>
+        <v>155</v>
       </c>
       <c r="F81" s="50">
         <v>1</v>
@@ -3811,16 +3811,16 @@
     </row>
     <row r="82" spans="1:7">
       <c r="A82" s="50" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="B82" s="50" t="s">
-        <v>194</v>
+        <v>162</v>
       </c>
       <c r="D82" s="56" t="s">
-        <v>176</v>
+        <v>144</v>
       </c>
       <c r="E82" s="50" t="s">
-        <v>184</v>
+        <v>152</v>
       </c>
       <c r="F82" s="50">
         <v>1</v>
@@ -3828,16 +3828,16 @@
     </row>
     <row r="83" spans="1:7">
       <c r="A83" s="50" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="B83" s="50" t="s">
-        <v>195</v>
+        <v>163</v>
       </c>
       <c r="D83" s="51" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="E83" s="50" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="F83" s="50">
         <v>1</v>
@@ -3845,16 +3845,16 @@
     </row>
     <row r="84" spans="1:7">
       <c r="A84" s="50" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="B84" s="50" t="s">
-        <v>196</v>
+        <v>164</v>
       </c>
       <c r="D84" s="51" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="E84" s="50" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="F84" s="50">
         <v>1</v>
@@ -3862,16 +3862,16 @@
     </row>
     <row r="85" spans="1:7">
       <c r="A85" s="50" t="s">
+        <v>133</v>
+      </c>
+      <c r="B85" s="50" t="s">
         <v>165</v>
       </c>
-      <c r="B85" s="50" t="s">
-        <v>197</v>
-      </c>
       <c r="D85" s="51" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="E85" s="50" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="F85" s="50">
         <v>1</v>
@@ -3879,42 +3879,42 @@
     </row>
     <row r="86" spans="1:7">
       <c r="A86" s="50" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="B86" s="50" t="s">
-        <v>198</v>
+        <v>166</v>
       </c>
       <c r="C86" s="50" t="s">
-        <v>134</v>
+        <v>102</v>
       </c>
       <c r="D86" s="50" t="s">
-        <v>199</v>
+        <v>167</v>
       </c>
       <c r="E86" s="50" t="s">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="F86" s="50">
         <v>1</v>
       </c>
       <c r="G86" s="50" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
     </row>
     <row r="87" spans="1:7">
       <c r="A87" s="50" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="B87" s="50" t="s">
-        <v>200</v>
+        <v>168</v>
       </c>
       <c r="C87" s="50" t="s">
-        <v>134</v>
+        <v>102</v>
       </c>
       <c r="D87" s="50" t="s">
-        <v>191</v>
+        <v>159</v>
       </c>
       <c r="E87" s="50" t="s">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="F87" s="50">
         <v>1</v>
@@ -3922,16 +3922,16 @@
     </row>
     <row r="88" spans="1:7">
       <c r="A88" s="50" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="B88" s="50" t="s">
-        <v>201</v>
+        <v>169</v>
       </c>
       <c r="D88" s="55" t="s">
-        <v>157</v>
+        <v>125</v>
       </c>
       <c r="E88" s="50" t="s">
-        <v>158</v>
+        <v>126</v>
       </c>
       <c r="F88" s="50">
         <v>1</v>
@@ -3939,16 +3939,16 @@
     </row>
     <row r="89" spans="1:7">
       <c r="A89" s="50" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="B89" s="50" t="s">
-        <v>202</v>
+        <v>170</v>
       </c>
       <c r="D89" s="55" t="s">
-        <v>157</v>
+        <v>125</v>
       </c>
       <c r="E89" s="50" t="s">
-        <v>158</v>
+        <v>126</v>
       </c>
       <c r="F89" s="50">
         <v>1</v>
@@ -3961,6 +3961,7 @@
       <c r="D91" s="58"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G1"/>
   <phoneticPr fontId="22" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3968,52 +3969,190 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:B19"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="11.42578125" style="45"/>
+    <col min="1" max="1" width="20.7109375" style="45" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="45" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" style="45" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="45"/>
+    <col min="5" max="5" width="20.5703125" style="45" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="45"/>
+    <col min="7" max="7" width="3.42578125" style="45" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="45"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:2">
-      <c r="B4" s="46"/>
-    </row>
-    <row r="5" spans="2:2">
-      <c r="B5" s="47"/>
-    </row>
-    <row r="6" spans="2:2">
+    <row r="1" spans="1:8">
+      <c r="A1" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="D1" s="48" t="s">
+        <v>174</v>
+      </c>
+      <c r="E1" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="49" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="49"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="45" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>182</v>
+      </c>
+      <c r="D2" s="45" t="s">
+        <v>176</v>
+      </c>
+      <c r="E2" s="45" t="s">
+        <v>210</v>
+      </c>
+      <c r="F2" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="45" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="45" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>182</v>
+      </c>
+      <c r="D3" s="45" t="s">
+        <v>176</v>
+      </c>
+      <c r="E3" s="45" t="s">
+        <v>210</v>
+      </c>
+      <c r="F3" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="45" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="45" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4" s="46" t="s">
+        <v>177</v>
+      </c>
+      <c r="C4" s="45" t="s">
+        <v>181</v>
+      </c>
+      <c r="D4" s="45" t="s">
+        <v>178</v>
+      </c>
+      <c r="E4" s="45" t="s">
+        <v>209</v>
+      </c>
+      <c r="F4" s="50" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="45" t="s">
+        <v>171</v>
+      </c>
+      <c r="B5" s="46" t="s">
+        <v>179</v>
+      </c>
+      <c r="C5" s="45" t="s">
+        <v>180</v>
+      </c>
+      <c r="D5" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="45" t="s">
+        <v>209</v>
+      </c>
+      <c r="F5" s="50" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="B6" s="47"/>
     </row>
-    <row r="7" spans="2:2">
+    <row r="7" spans="1:8">
       <c r="B7" s="47"/>
     </row>
-    <row r="8" spans="2:2">
+    <row r="8" spans="1:8">
       <c r="B8" s="47"/>
     </row>
-    <row r="9" spans="2:2">
+    <row r="9" spans="1:8">
       <c r="B9" s="47"/>
     </row>
-    <row r="10" spans="2:2">
+    <row r="10" spans="1:8">
       <c r="B10" s="47"/>
     </row>
-    <row r="11" spans="2:2">
-      <c r="B11" s="47"/>
-    </row>
-    <row r="12" spans="2:2">
-      <c r="B12" s="47"/>
-    </row>
-    <row r="13" spans="2:2">
-      <c r="B13" s="47"/>
-    </row>
-    <row r="14" spans="2:2">
+    <row r="11" spans="1:8">
+      <c r="A11" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="48" t="s">
+        <v>198</v>
+      </c>
+      <c r="C11" s="48" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="45" t="s">
+        <v>209</v>
+      </c>
+      <c r="B12" s="47" t="s">
+        <v>208</v>
+      </c>
+      <c r="C12" s="45" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="45" t="s">
+        <v>210</v>
+      </c>
+      <c r="B13" s="47" t="s">
+        <v>206</v>
+      </c>
+      <c r="C13" s="45" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="B14" s="47"/>
     </row>
-    <row r="15" spans="2:2">
+    <row r="15" spans="1:8">
       <c r="B15" s="47"/>
     </row>
-    <row r="16" spans="2:2">
+    <row r="16" spans="1:8">
       <c r="B16" s="47"/>
     </row>
     <row r="17" spans="2:2">
@@ -4026,6 +4165,7 @@
       <c r="B19" s="47"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G1"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4033,177 +4173,197 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B27"/>
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A19" sqref="A1:C1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="44" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" style="44" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2">
+    <row r="1" spans="1:6">
+      <c r="A1" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="48" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="49" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>186</v>
       </c>
       <c r="B2" s="44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="60">
+        <v>183</v>
+      </c>
+      <c r="C2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E2" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E3" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>188</v>
+      </c>
+      <c r="C4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D4" t="s">
+        <v>190</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C5" t="s">
+        <v>196</v>
+      </c>
+      <c r="D5" t="s">
+        <v>193</v>
+      </c>
+      <c r="E5" s="50" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C6" t="s">
+        <v>196</v>
+      </c>
+      <c r="D6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E6" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="B7"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="B9"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="44" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="375">
-      <c r="A4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="44" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="165">
-      <c r="A5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="44" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="409.5">
-      <c r="A6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="44" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="45">
-      <c r="A7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="44" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="165">
-      <c r="A8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="44" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="180">
-      <c r="A9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="44" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="30">
-      <c r="A10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="44" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="45">
+      <c r="B10" s="48" t="s">
+        <v>198</v>
+      </c>
+      <c r="C10" s="48" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>193</v>
       </c>
       <c r="B11" s="44" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="60">
+        <v>199</v>
+      </c>
+      <c r="C11" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="B12" s="44" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="345">
+        <v>202</v>
+      </c>
+      <c r="C12" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>190</v>
       </c>
       <c r="B13" s="44" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="150">
-      <c r="A14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B14" s="44" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="150">
-      <c r="A15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15" s="44" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="30">
-      <c r="A16" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" s="44" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="30">
-      <c r="A17" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="44" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="30">
-      <c r="A18" t="s">
-        <v>63</v>
-      </c>
-      <c r="B18" s="44" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="B21"/>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="B22"/>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="B23"/>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="B24"/>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="B25"/>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="B26"/>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="B27"/>
+        <v>203</v>
+      </c>
+      <c r="C13" t="s">
+        <v>204</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F1"/>
+  <sortState ref="A2:F6">
+    <sortCondition ref="A2:A6"/>
+    <sortCondition ref="B2:B6"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>